<commit_message>
format data to .00 and added Normal 3-people data
</commit_message>
<xml_diff>
--- a/Data/3/NewYear-3-Processed.xlsx
+++ b/Data/3/NewYear-3-Processed.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\si140\PJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\si140\PJ\SI140A-proj\Data\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F635C-8D05-4574-95D7-E8C1F1FA5392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D5273B-E6F1-4090-9509-452444C88108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="红包收入" sheetId="1" r:id="rId1"/>
-    <sheet name="红包数据统计" sheetId="2" r:id="rId2"/>
+    <sheet name="Received" sheetId="2" r:id="rId1"/>
+    <sheet name="TotalLeft" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,27 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
-  <si>
-    <t>昵称</t>
-  </si>
-  <si>
-    <t>红包总收入</t>
-  </si>
-  <si>
-    <t>红包总支出</t>
-  </si>
-  <si>
-    <t>补偿数额</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>钱磊</t>
-  </si>
-  <si>
-    <t>zzh</t>
-  </si>
-  <si>
-    <t>xjq</t>
   </si>
   <si>
     <t>发送者</t>
@@ -114,11 +96,26 @@
     <t>Count</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Sender</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red Envelope receive rank</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Money</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -199,6 +196,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -209,27 +224,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -298,7 +295,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>红包数据统计!$H$5:$H$10</c:f>
+              <c:f>Received!$H$5:$H$10</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -324,7 +321,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>红包数据统计!$I$5:$I$10</c:f>
+              <c:f>Received!$I$5:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -491,7 +488,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>红包数据统计!$H$16:$H$21</c:f>
+              <c:f>Received!$H$16:$H$21</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -517,7 +514,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>红包数据统计!$I$16:$I$21</c:f>
+              <c:f>Received!$I$16:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -681,7 +678,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>红包数据统计!$H$27:$H$32</c:f>
+              <c:f>Received!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -707,7 +704,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>红包数据统计!$I$27:$I$32</c:f>
+              <c:f>Received!$I$27:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1172,107 +1169,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="红包收入"/>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.15234375" defaultRowHeight="18" customHeight="1"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1339.54</v>
-      </c>
-      <c r="C2">
-        <v>1200</v>
-      </c>
-      <c r="D2">
-        <f>-B2+C2</f>
-        <v>-139.53999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1258.3</v>
-      </c>
-      <c r="C3">
-        <v>1200</v>
-      </c>
-      <c r="D3">
-        <f>-B3+C3</f>
-        <v>-58.299999999999955</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1200</v>
-      </c>
-      <c r="D4">
-        <f>-B4+C4</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
-        <v>2597.84</v>
-      </c>
-      <c r="C5">
-        <f>SUM(C2:C4)</f>
-        <v>3600</v>
-      </c>
-      <c r="D5">
-        <f>SUM(D2:D4)</f>
-        <v>1002.1600000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="红包数据统计"/>
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.15234375" defaultRowHeight="18" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1283,8 +1195,8 @@
       <c r="E1">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>11</v>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="H1">
         <v>10</v>
@@ -1303,19 +1215,19 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
+      <c r="A2" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="14">
         <v>26.77</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="14">
         <v>26.68</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="14">
         <v>6.55</v>
       </c>
       <c r="F2">
@@ -1324,17 +1236,17 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="11"/>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="14">
         <v>37.01</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="14">
         <v>9.89</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="14">
         <v>13.1</v>
       </c>
       <c r="F3">
@@ -1343,192 +1255,192 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="11"/>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="14">
         <v>19.829999999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="14">
         <v>23.87</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="14">
         <v>16.3</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>22</v>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="14">
         <v>29.88</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="14">
         <v>29.48</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="14">
         <v>0.64</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="I5" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="14">
         <v>21.3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="14">
         <v>12.21</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>26.49</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="H6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="14">
         <v>22.35</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="14">
         <v>28.6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="14">
         <v>9.0500000000000007</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="H7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="14">
         <v>7.17</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="14">
         <v>47.27</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="14">
         <v>5.56</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>60.000000000000007</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="H8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18" customHeight="1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="14">
         <v>28.77</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="14">
         <v>24.38</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="14">
         <v>6.85</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="H9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="11"/>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="14">
         <v>10.34</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="14">
         <v>31</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="14">
         <v>18.66</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="11"/>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="14">
         <v>39.880000000000003</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="14">
         <v>5.83</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="14">
         <v>14.29</v>
       </c>
       <c r="F11">
@@ -1537,19 +1449,19 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>9</v>
+      <c r="A12" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="14">
         <v>38.85</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="14">
         <v>17.39</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="14">
         <v>3.76</v>
       </c>
       <c r="F12">
@@ -1559,17 +1471,17 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="11"/>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="14">
         <v>24.71</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="14">
         <v>30.44</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="14">
         <v>4.8499999999999996</v>
       </c>
       <c r="F13">
@@ -1579,17 +1491,17 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="11"/>
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="14">
         <v>9.11</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="14">
         <v>25.66</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="14">
         <v>25.23</v>
       </c>
       <c r="F14">
@@ -1599,17 +1511,17 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="11"/>
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="14">
         <v>13.93</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="14">
         <v>44.21</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="14">
         <v>1.86</v>
       </c>
       <c r="F15">
@@ -1617,25 +1529,25 @@
         <v>60</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>22</v>
+      <c r="H15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="14">
         <v>25.77</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="14">
         <v>1.71</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="14">
         <v>32.520000000000003</v>
       </c>
       <c r="F16">
@@ -1643,25 +1555,25 @@
         <v>60</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3">
         <v>17</v>
       </c>
-      <c r="I16" s="10">
-        <v>17</v>
-      </c>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="11"/>
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="14">
         <v>19.22</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="14">
         <v>30.39</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="14">
         <v>10.39</v>
       </c>
       <c r="F17">
@@ -1669,25 +1581,25 @@
         <v>60</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="10">
+      <c r="H17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="11"/>
       <c r="B18">
         <v>7</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="14">
         <v>21.04</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="14">
         <v>3.76</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="14">
         <v>35.200000000000003</v>
       </c>
       <c r="F18">
@@ -1695,25 +1607,25 @@
         <v>60</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="10">
+      <c r="H18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1">
-      <c r="A19" s="5"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>8</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="14">
         <v>36.14</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="14">
         <v>19.25</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="14">
         <v>4.6100000000000003</v>
       </c>
       <c r="F19">
@@ -1721,25 +1633,25 @@
         <v>60</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="10">
+      <c r="H19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1">
-      <c r="A20" s="5"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>9</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="14">
         <v>38.82</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="14">
         <v>17.41</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="14">
         <v>3.77</v>
       </c>
       <c r="F20">
@@ -1747,25 +1659,25 @@
         <v>60.000000000000007</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="10">
+      <c r="H20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" thickBot="1">
-      <c r="A21" s="5"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="14">
         <v>18.37</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="14">
         <v>14.97</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="14">
         <v>26.66</v>
       </c>
       <c r="F21">
@@ -1773,27 +1685,27 @@
         <v>60</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="11">
+      <c r="H21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16.5">
-      <c r="A22" s="4" t="s">
-        <v>4</v>
+      <c r="A22" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="14">
         <v>18.22</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="14">
         <v>9.69</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="14">
         <v>32.090000000000003</v>
       </c>
       <c r="F22">
@@ -1802,17 +1714,17 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="16.5">
-      <c r="A23" s="5"/>
+      <c r="A23" s="11"/>
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="14">
         <v>8.7799999999999994</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="14">
         <v>35.119999999999997</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="14">
         <v>16.100000000000001</v>
       </c>
       <c r="F23">
@@ -1821,17 +1733,17 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="16.5">
-      <c r="A24" s="5"/>
+      <c r="A24" s="11"/>
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="14">
         <v>14.15</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="14">
         <v>2.98</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="14">
         <v>42.87</v>
       </c>
       <c r="F24">
@@ -1840,17 +1752,17 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="17" thickBot="1">
-      <c r="A25" s="5"/>
+      <c r="A25" s="11"/>
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="14">
         <v>29.54</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="14">
         <v>14.21</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="14">
         <v>16.25</v>
       </c>
       <c r="F25">
@@ -1859,194 +1771,194 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="16.5">
-      <c r="A26" s="5"/>
+      <c r="A26" s="11"/>
       <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="14">
         <v>22.21</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="14">
         <v>15.4</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="14">
         <v>22.39</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>22</v>
+      <c r="H26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="16.5">
-      <c r="A27" s="5"/>
+      <c r="A27" s="11"/>
       <c r="B27">
         <v>6</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="14">
         <v>21.97</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="14">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="14">
         <v>33.130000000000003</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="10">
+      <c r="H27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16.5">
-      <c r="A28" s="5"/>
+      <c r="A28" s="11"/>
       <c r="B28">
         <v>7</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="14">
         <v>13.64</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="14">
         <v>14.16</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="14">
         <v>32.200000000000003</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="10">
+      <c r="H28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="3">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="16.5">
-      <c r="A29" s="5"/>
+      <c r="A29" s="11"/>
       <c r="B29">
         <v>8</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="14">
         <v>8.3699999999999992</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="14">
         <v>36.479999999999997</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="14">
         <v>15.15</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>59.999999999999993</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="10">
+      <c r="H29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="16.5">
-      <c r="A30" s="5"/>
+      <c r="A30" s="11"/>
       <c r="B30">
         <v>9</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="14">
         <v>2.62</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="14">
         <v>38.33</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="14">
         <v>19.05</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="10">
+      <c r="H30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16.5">
-      <c r="A31" s="5"/>
+      <c r="A31" s="11"/>
       <c r="B31">
         <v>10</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="14">
         <v>36.659999999999997</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="14">
         <v>6.12</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="14">
         <v>17.22</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>59.999999999999993</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="10">
+      <c r="H31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17" thickBot="1">
-      <c r="A32" s="4" t="s">
-        <v>9</v>
+      <c r="A32" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="14">
         <v>15.52</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="14">
         <v>17.75</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="14">
         <v>26.73</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H32" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="11">
+      <c r="H32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5">
-      <c r="A33" s="5"/>
+      <c r="A33" s="11"/>
       <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="14">
         <v>30.49</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="14">
         <v>16.690000000000001</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="14">
         <v>12.82</v>
       </c>
       <c r="F33">
@@ -2055,17 +1967,17 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16.5">
-      <c r="A34" s="5"/>
+      <c r="A34" s="11"/>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="14">
         <v>19.829999999999998</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="14">
         <v>16.32</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="14">
         <v>23.85</v>
       </c>
       <c r="F34">
@@ -2074,17 +1986,17 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="16.5">
-      <c r="A35" s="5"/>
+      <c r="A35" s="11"/>
       <c r="B35">
         <v>4</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="14">
         <v>8.3699999999999992</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="14">
         <v>2.58</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="14">
         <v>49.05</v>
       </c>
       <c r="F35">
@@ -2093,17 +2005,17 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="16.5">
-      <c r="A36" s="5"/>
+      <c r="A36" s="11"/>
       <c r="B36">
         <v>5</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="14">
         <v>6.75</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="14">
         <v>53.1</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="14">
         <v>0.15</v>
       </c>
       <c r="F36">
@@ -2112,17 +2024,17 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="16.5">
-      <c r="A37" s="5"/>
+      <c r="A37" s="11"/>
       <c r="B37">
         <v>6</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="14">
         <v>26.07</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="14">
         <v>23.11</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="14">
         <v>10.82</v>
       </c>
       <c r="F37">
@@ -2131,17 +2043,17 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="16.5">
-      <c r="A38" s="5"/>
+      <c r="A38" s="11"/>
       <c r="B38">
         <v>7</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="14">
         <v>34.32</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="14">
         <v>12.4</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="14">
         <v>13.28</v>
       </c>
       <c r="F38">
@@ -2150,17 +2062,17 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5">
-      <c r="A39" s="5"/>
+      <c r="A39" s="11"/>
       <c r="B39">
         <v>8</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="14">
         <v>29.84</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="14">
         <v>21.09</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="14">
         <v>9.07</v>
       </c>
       <c r="F39">
@@ -2169,17 +2081,17 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5">
-      <c r="A40" s="5"/>
+      <c r="A40" s="11"/>
       <c r="B40">
         <v>9</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="14">
         <v>25.96</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="14">
         <v>16.45</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="14">
         <v>17.59</v>
       </c>
       <c r="F40">
@@ -2188,17 +2100,17 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.5">
-      <c r="A41" s="5"/>
+      <c r="A41" s="11"/>
       <c r="B41">
         <v>10</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="14">
         <v>25.07</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="14">
         <v>19.600000000000001</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="14">
         <v>15.33</v>
       </c>
       <c r="F41">
@@ -2207,19 +2119,19 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="16.5">
-      <c r="A42" s="4" t="s">
-        <v>10</v>
+      <c r="A42" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="14">
         <v>7.95</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="14">
         <v>16.41</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="14">
         <v>35.64</v>
       </c>
       <c r="F42">
@@ -2228,17 +2140,17 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5">
-      <c r="A43" s="5"/>
+      <c r="A43" s="11"/>
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="14">
         <v>33.79</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="14">
         <v>22.41</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="14">
         <v>3.8</v>
       </c>
       <c r="F43">
@@ -2247,17 +2159,17 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="16.5">
-      <c r="A44" s="5"/>
+      <c r="A44" s="11"/>
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="14">
         <v>11.71</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="14">
         <v>32.64</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="14">
         <v>15.65</v>
       </c>
       <c r="F44">
@@ -2266,17 +2178,17 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5">
-      <c r="A45" s="5"/>
+      <c r="A45" s="11"/>
       <c r="B45">
         <v>4</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="14">
         <v>2.68</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="14">
         <v>38.950000000000003</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="14">
         <v>18.37</v>
       </c>
       <c r="F45">
@@ -2285,17 +2197,17 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5">
-      <c r="A46" s="5"/>
+      <c r="A46" s="11"/>
       <c r="B46">
         <v>5</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="14">
         <v>33.07</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="14">
         <v>7.39</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="14">
         <v>19.54</v>
       </c>
       <c r="F46">
@@ -2304,17 +2216,17 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5">
-      <c r="A47" s="5"/>
+      <c r="A47" s="11"/>
       <c r="B47">
         <v>6</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="14">
         <v>20.51</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="14">
         <v>31.52</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="14">
         <v>7.97</v>
       </c>
       <c r="F47">
@@ -2323,17 +2235,17 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5">
-      <c r="A48" s="5"/>
+      <c r="A48" s="11"/>
       <c r="B48">
         <v>7</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="14">
         <v>19.79</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="14">
         <v>28.33</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="14">
         <v>11.88</v>
       </c>
       <c r="F48">
@@ -2342,17 +2254,17 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5">
-      <c r="A49" s="5"/>
+      <c r="A49" s="11"/>
       <c r="B49">
         <v>8</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="14">
         <v>6.29</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="14">
         <v>16.510000000000002</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="14">
         <v>37.200000000000003</v>
       </c>
       <c r="F49">
@@ -2361,17 +2273,17 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5">
-      <c r="A50" s="5"/>
+      <c r="A50" s="11"/>
       <c r="B50">
         <v>9</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="14">
         <v>16.2</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="14">
         <v>5.78</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="14">
         <v>38.020000000000003</v>
       </c>
       <c r="F50">
@@ -2380,17 +2292,17 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5">
-      <c r="A51" s="5"/>
+      <c r="A51" s="11"/>
       <c r="B51">
         <v>10</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="14">
         <v>2</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="14">
         <v>5.47</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="14">
         <v>52.53</v>
       </c>
       <c r="F51">
@@ -2399,18 +2311,18 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5">
-      <c r="A52" s="5"/>
+      <c r="A52" s="11"/>
       <c r="B52">
         <f t="shared" ref="B52:B61" si="1">B42+10</f>
         <v>11</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="14">
         <v>31.86</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="14">
         <v>24.54</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="14">
         <v>3.6</v>
       </c>
       <c r="F52">
@@ -2419,18 +2331,18 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="16.5">
-      <c r="A53" s="5"/>
+      <c r="A53" s="11"/>
       <c r="B53">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="14">
         <v>12.37</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="14">
         <v>8.98</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="14">
         <v>38.65</v>
       </c>
       <c r="F53">
@@ -2439,18 +2351,18 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="16.5">
-      <c r="A54" s="5"/>
+      <c r="A54" s="11"/>
       <c r="B54">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="14">
         <v>19.29</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="14">
         <v>23.16</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="14">
         <v>17.55</v>
       </c>
       <c r="F54">
@@ -2459,18 +2371,18 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.5">
-      <c r="A55" s="5"/>
+      <c r="A55" s="11"/>
       <c r="B55">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="14">
         <v>17.149999999999999</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="14">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="14">
         <v>38.49</v>
       </c>
       <c r="F55">
@@ -2479,18 +2391,18 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="16.5">
-      <c r="A56" s="5"/>
+      <c r="A56" s="11"/>
       <c r="B56">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="14">
         <v>12.49</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="14">
         <v>21.57</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="14">
         <v>25.94</v>
       </c>
       <c r="F56">
@@ -2499,18 +2411,18 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="16.5">
-      <c r="A57" s="5"/>
+      <c r="A57" s="11"/>
       <c r="B57">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="14">
         <v>38.159999999999997</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="14">
         <v>5.28</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="14">
         <v>16.559999999999999</v>
       </c>
       <c r="F57">
@@ -2519,18 +2431,18 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="16.5">
-      <c r="A58" s="5"/>
+      <c r="A58" s="11"/>
       <c r="B58">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="14">
         <v>20.25</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="14">
         <v>6.26</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="14">
         <v>33.49</v>
       </c>
       <c r="F58">
@@ -2539,18 +2451,18 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="16.5">
-      <c r="A59" s="5"/>
+      <c r="A59" s="11"/>
       <c r="B59">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="14">
         <v>31.78</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="14">
         <v>9.15</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="14">
         <v>19.07</v>
       </c>
       <c r="F59">
@@ -2559,18 +2471,18 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="16.5">
-      <c r="A60" s="5"/>
+      <c r="A60" s="11"/>
       <c r="B60">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="14">
         <v>14.37</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="14">
         <v>33.33</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="14">
         <v>12.3</v>
       </c>
       <c r="F60">
@@ -2579,18 +2491,18 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="16.5">
-      <c r="A61" s="5"/>
+      <c r="A61" s="11"/>
       <c r="B61">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="14">
         <v>37.89</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="14">
         <v>17.52</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="14">
         <v>4.59</v>
       </c>
       <c r="F61">
@@ -2599,111 +2511,52 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="18" customHeight="1">
-      <c r="A62" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>13</v>
+      <c r="A62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C62">
         <f>AVERAGE(C2:C61)</f>
         <v>21.287333333333333</v>
       </c>
       <c r="D62">
-        <f t="shared" ref="D62:F62" si="2">AVERAGE(D2:D61)</f>
+        <f t="shared" ref="D62:E62" si="2">AVERAGE(D2:D61)</f>
         <v>19.673999999999999</v>
       </c>
       <c r="E62">
         <f t="shared" si="2"/>
         <v>19.038666666666664</v>
       </c>
-      <c r="F62" s="8" t="s">
-        <v>13</v>
+      <c r="F62" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="18" customHeight="1">
-      <c r="A63" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>13</v>
+      <c r="A63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C63">
         <f>VAR(C2:C61)</f>
         <v>111.88301649717515</v>
       </c>
       <c r="D63">
-        <f t="shared" ref="D63:F63" si="3">VAR(D2:D61)</f>
+        <f t="shared" ref="D63:E63" si="3">VAR(D2:D61)</f>
         <v>146.08965491525436</v>
       </c>
       <c r="E63">
         <f t="shared" si="3"/>
         <v>162.83363548022601</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="16.5">
-      <c r="A65" s="9"/>
-    </row>
-    <row r="66" spans="1:1" ht="18" customHeight="1">
-      <c r="A66" s="9"/>
-    </row>
-    <row r="67" spans="1:1" ht="18" customHeight="1">
-      <c r="A67" s="9"/>
-    </row>
-    <row r="68" spans="1:1" ht="18" customHeight="1">
-      <c r="A68" s="9"/>
-    </row>
-    <row r="69" spans="1:1" ht="18" customHeight="1">
-      <c r="A69" s="9"/>
-    </row>
-    <row r="70" spans="1:1" ht="18" customHeight="1">
-      <c r="A70" s="9"/>
-    </row>
-    <row r="71" spans="1:1" ht="18" customHeight="1">
-      <c r="A71" s="9"/>
-    </row>
-    <row r="72" spans="1:1" ht="18" customHeight="1">
-      <c r="A72" s="9"/>
-    </row>
-    <row r="73" spans="1:1" ht="18" customHeight="1">
-      <c r="A73" s="9"/>
-    </row>
-    <row r="74" spans="1:1" ht="18" customHeight="1">
-      <c r="A74" s="9"/>
-    </row>
-    <row r="75" spans="1:1" ht="18" customHeight="1">
-      <c r="A75" s="9"/>
-    </row>
-    <row r="76" spans="1:1" ht="18" customHeight="1">
-      <c r="A76" s="9"/>
-    </row>
-    <row r="77" spans="1:1" ht="18" customHeight="1">
-      <c r="A77" s="9"/>
-    </row>
-    <row r="78" spans="1:1" ht="18" customHeight="1">
-      <c r="A78" s="9"/>
-    </row>
-    <row r="79" spans="1:1" ht="18" customHeight="1">
-      <c r="A79" s="9"/>
-    </row>
-    <row r="80" spans="1:1" ht="18" customHeight="1">
-      <c r="A80" s="9"/>
-    </row>
-    <row r="81" spans="1:1" ht="18" customHeight="1">
-      <c r="A81" s="9"/>
-    </row>
-    <row r="82" spans="1:1" ht="18" customHeight="1">
-      <c r="A82" s="9"/>
-    </row>
-    <row r="83" spans="1:1" ht="18" customHeight="1">
-      <c r="A83" s="9"/>
-    </row>
-    <row r="84" spans="1:1" ht="18" customHeight="1">
-      <c r="A84" s="9"/>
-    </row>
+      <c r="F63" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" ht="16.5"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H27:H31">
     <sortCondition ref="H27"/>
@@ -2723,4 +2576,1342 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223FD66D-FA6D-45F1-AF5A-A4BC1C8FC9D8}">
+  <dimension ref="A1:F63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="22.765625" customWidth="1"/>
+    <col min="6" max="6" width="11.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
+        <f>60-Received!C2</f>
+        <v>33.230000000000004</v>
+      </c>
+      <c r="D2" s="14">
+        <f>C2-Received!D2</f>
+        <v>6.5500000000000043</v>
+      </c>
+      <c r="E2" s="14">
+        <f>D2-Received!E2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="11"/>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <f>60-Received!C3</f>
+        <v>22.990000000000002</v>
+      </c>
+      <c r="D3" s="14">
+        <f>C3-Received!D3</f>
+        <v>13.100000000000001</v>
+      </c>
+      <c r="E3" s="14">
+        <f>D3-Received!E3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11"/>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14">
+        <f>60-Received!C4</f>
+        <v>40.17</v>
+      </c>
+      <c r="D4" s="14">
+        <f>C4-Received!D4</f>
+        <v>16.3</v>
+      </c>
+      <c r="E4" s="14">
+        <f>D4-Received!E4</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11"/>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="14">
+        <f>60-Received!C5</f>
+        <v>30.12</v>
+      </c>
+      <c r="D5" s="14">
+        <f>C5-Received!D5</f>
+        <v>0.64000000000000057</v>
+      </c>
+      <c r="E5" s="14">
+        <f>D5-Received!E5</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="11"/>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="14">
+        <f>60-Received!C6</f>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="D6" s="14">
+        <f>C6-Received!D6</f>
+        <v>26.490000000000002</v>
+      </c>
+      <c r="E6" s="14">
+        <f>D6-Received!E6</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="11"/>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14">
+        <f>60-Received!C7</f>
+        <v>37.65</v>
+      </c>
+      <c r="D7" s="14">
+        <f>C7-Received!D7</f>
+        <v>9.0499999999999972</v>
+      </c>
+      <c r="E7" s="14">
+        <f>D7-Received!E7</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11"/>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14">
+        <f>60-Received!C8</f>
+        <v>52.83</v>
+      </c>
+      <c r="D8" s="14">
+        <f>C8-Received!D8</f>
+        <v>5.5599999999999952</v>
+      </c>
+      <c r="E8" s="14">
+        <f>D8-Received!E8</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="11"/>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14">
+        <f>60-Received!C9</f>
+        <v>31.23</v>
+      </c>
+      <c r="D9" s="14">
+        <f>C9-Received!D9</f>
+        <v>6.8500000000000014</v>
+      </c>
+      <c r="E9" s="14">
+        <f>D9-Received!E9</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="11"/>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14">
+        <f>60-Received!C10</f>
+        <v>49.66</v>
+      </c>
+      <c r="D10" s="14">
+        <f>C10-Received!D10</f>
+        <v>18.659999999999997</v>
+      </c>
+      <c r="E10" s="14">
+        <f>D10-Received!E10</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="11"/>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14">
+        <f>60-Received!C11</f>
+        <v>20.119999999999997</v>
+      </c>
+      <c r="D11" s="14">
+        <f>C11-Received!D11</f>
+        <v>14.289999999999997</v>
+      </c>
+      <c r="E11" s="14">
+        <f>D11-Received!E11</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
+        <f>60-Received!C12</f>
+        <v>21.15</v>
+      </c>
+      <c r="D12" s="14">
+        <f>C12-Received!D12</f>
+        <v>3.759999999999998</v>
+      </c>
+      <c r="E12" s="14">
+        <f>D12-Received!E12</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="11"/>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="14">
+        <f>60-Received!C13</f>
+        <v>35.29</v>
+      </c>
+      <c r="D13" s="14">
+        <f>C13-Received!D13</f>
+        <v>4.8499999999999979</v>
+      </c>
+      <c r="E13" s="14">
+        <f>D13-Received!E13</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="11"/>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14">
+        <f>60-Received!C14</f>
+        <v>50.89</v>
+      </c>
+      <c r="D14" s="14">
+        <f>C14-Received!D14</f>
+        <v>25.23</v>
+      </c>
+      <c r="E14" s="14">
+        <f>D14-Received!E14</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="11"/>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14">
+        <f>60-Received!C15</f>
+        <v>46.07</v>
+      </c>
+      <c r="D15" s="14">
+        <f>C15-Received!D15</f>
+        <v>1.8599999999999994</v>
+      </c>
+      <c r="E15" s="14">
+        <f>D15-Received!E15</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="11"/>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" s="14">
+        <f>60-Received!C16</f>
+        <v>34.230000000000004</v>
+      </c>
+      <c r="D16" s="14">
+        <f>C16-Received!D16</f>
+        <v>32.520000000000003</v>
+      </c>
+      <c r="E16" s="14">
+        <f>D16-Received!E16</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="11"/>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" s="14">
+        <f>60-Received!C17</f>
+        <v>40.78</v>
+      </c>
+      <c r="D17" s="14">
+        <f>C17-Received!D17</f>
+        <v>10.39</v>
+      </c>
+      <c r="E17" s="14">
+        <f>D17-Received!E17</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="11"/>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" s="14">
+        <f>60-Received!C18</f>
+        <v>38.96</v>
+      </c>
+      <c r="D18" s="14">
+        <f>C18-Received!D18</f>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E18" s="14">
+        <f>D18-Received!E18</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="11"/>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" s="14">
+        <f>60-Received!C19</f>
+        <v>23.86</v>
+      </c>
+      <c r="D19" s="14">
+        <f>C19-Received!D19</f>
+        <v>4.6099999999999994</v>
+      </c>
+      <c r="E19" s="14">
+        <f>D19-Received!E19</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="11"/>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20" s="14">
+        <f>60-Received!C20</f>
+        <v>21.18</v>
+      </c>
+      <c r="D20" s="14">
+        <f>C20-Received!D20</f>
+        <v>3.7699999999999996</v>
+      </c>
+      <c r="E20" s="14">
+        <f>D20-Received!E20</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="11"/>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" s="14">
+        <f>60-Received!C21</f>
+        <v>41.629999999999995</v>
+      </c>
+      <c r="D21" s="14">
+        <f>C21-Received!D21</f>
+        <v>26.659999999999997</v>
+      </c>
+      <c r="E21" s="14">
+        <f>D21-Received!E21</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="14">
+        <f>60-Received!C22</f>
+        <v>41.78</v>
+      </c>
+      <c r="D22" s="14">
+        <f>C22-Received!D22</f>
+        <v>32.090000000000003</v>
+      </c>
+      <c r="E22" s="14">
+        <f>D22-Received!E22</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="11"/>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="14">
+        <f>60-Received!C23</f>
+        <v>51.22</v>
+      </c>
+      <c r="D23" s="14">
+        <f>C23-Received!D23</f>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E23" s="14">
+        <f>D23-Received!E23</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="11"/>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="14">
+        <f>60-Received!C24</f>
+        <v>45.85</v>
+      </c>
+      <c r="D24" s="14">
+        <f>C24-Received!D24</f>
+        <v>42.870000000000005</v>
+      </c>
+      <c r="E24" s="14">
+        <f>D24-Received!E24</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="11"/>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="14">
+        <f>60-Received!C25</f>
+        <v>30.46</v>
+      </c>
+      <c r="D25" s="14">
+        <f>C25-Received!D25</f>
+        <v>16.25</v>
+      </c>
+      <c r="E25" s="14">
+        <f>D25-Received!E25</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="11"/>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" s="14">
+        <f>60-Received!C26</f>
+        <v>37.79</v>
+      </c>
+      <c r="D26" s="14">
+        <f>C26-Received!D26</f>
+        <v>22.39</v>
+      </c>
+      <c r="E26" s="14">
+        <f>D26-Received!E26</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="11"/>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" s="14">
+        <f>60-Received!C27</f>
+        <v>38.03</v>
+      </c>
+      <c r="D27" s="14">
+        <f>C27-Received!D27</f>
+        <v>33.130000000000003</v>
+      </c>
+      <c r="E27" s="14">
+        <f>D27-Received!E27</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="11"/>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" s="14">
+        <f>60-Received!C28</f>
+        <v>46.36</v>
+      </c>
+      <c r="D28" s="14">
+        <f>C28-Received!D28</f>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E28" s="14">
+        <f>D28-Received!E28</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="11"/>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" s="14">
+        <f>60-Received!C29</f>
+        <v>51.63</v>
+      </c>
+      <c r="D29" s="14">
+        <f>C29-Received!D29</f>
+        <v>15.150000000000006</v>
+      </c>
+      <c r="E29" s="14">
+        <f>D29-Received!E29</f>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="11"/>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30" s="14">
+        <f>60-Received!C30</f>
+        <v>57.38</v>
+      </c>
+      <c r="D30" s="14">
+        <f>C30-Received!D30</f>
+        <v>19.050000000000004</v>
+      </c>
+      <c r="E30" s="14">
+        <f>D30-Received!E30</f>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="11"/>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31" s="14">
+        <f>60-Received!C31</f>
+        <v>23.340000000000003</v>
+      </c>
+      <c r="D31" s="14">
+        <f>C31-Received!D31</f>
+        <v>17.220000000000002</v>
+      </c>
+      <c r="E31" s="14">
+        <f>D31-Received!E31</f>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14">
+        <f>60-Received!C32</f>
+        <v>44.480000000000004</v>
+      </c>
+      <c r="D32" s="14">
+        <f>C32-Received!D32</f>
+        <v>26.730000000000004</v>
+      </c>
+      <c r="E32" s="14">
+        <f>D32-Received!E32</f>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="11"/>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14">
+        <f>60-Received!C33</f>
+        <v>29.51</v>
+      </c>
+      <c r="D33" s="14">
+        <f>C33-Received!D33</f>
+        <v>12.82</v>
+      </c>
+      <c r="E33" s="14">
+        <f>D33-Received!E33</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="11"/>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" s="14">
+        <f>60-Received!C34</f>
+        <v>40.17</v>
+      </c>
+      <c r="D34" s="14">
+        <f>C34-Received!D34</f>
+        <v>23.85</v>
+      </c>
+      <c r="E34" s="14">
+        <f>D34-Received!E34</f>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="11"/>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" s="14">
+        <f>60-Received!C35</f>
+        <v>51.63</v>
+      </c>
+      <c r="D35" s="14">
+        <f>C35-Received!D35</f>
+        <v>49.050000000000004</v>
+      </c>
+      <c r="E35" s="14">
+        <f>D35-Received!E35</f>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="11"/>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" s="14">
+        <f>60-Received!C36</f>
+        <v>53.25</v>
+      </c>
+      <c r="D36" s="14">
+        <f>C36-Received!D36</f>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="E36" s="14">
+        <f>D36-Received!E36</f>
+        <v>-1.4155343563970746E-15</v>
+      </c>
+      <c r="F36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="11"/>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" s="14">
+        <f>60-Received!C37</f>
+        <v>33.93</v>
+      </c>
+      <c r="D37" s="14">
+        <f>C37-Received!D37</f>
+        <v>10.82</v>
+      </c>
+      <c r="E37" s="14">
+        <f>D37-Received!E37</f>
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="11"/>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" s="14">
+        <f>60-Received!C38</f>
+        <v>25.68</v>
+      </c>
+      <c r="D38" s="14">
+        <f>C38-Received!D38</f>
+        <v>13.28</v>
+      </c>
+      <c r="E38" s="14">
+        <f>D38-Received!E38</f>
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="11"/>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" s="14">
+        <f>60-Received!C39</f>
+        <v>30.16</v>
+      </c>
+      <c r="D39" s="14">
+        <f>C39-Received!D39</f>
+        <v>9.07</v>
+      </c>
+      <c r="E39" s="14">
+        <f>D39-Received!E39</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="11"/>
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40" s="14">
+        <f>60-Received!C40</f>
+        <v>34.04</v>
+      </c>
+      <c r="D40" s="14">
+        <f>C40-Received!D40</f>
+        <v>17.59</v>
+      </c>
+      <c r="E40" s="14">
+        <f>D40-Received!E40</f>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="11"/>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41" s="14">
+        <f>60-Received!C41</f>
+        <v>34.93</v>
+      </c>
+      <c r="D41" s="14">
+        <f>C41-Received!D41</f>
+        <v>15.329999999999998</v>
+      </c>
+      <c r="E41" s="14">
+        <f>D41-Received!E41</f>
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="14">
+        <f>60-Received!C42</f>
+        <v>52.05</v>
+      </c>
+      <c r="D42" s="14">
+        <f>C42-Received!D42</f>
+        <v>35.64</v>
+      </c>
+      <c r="E42" s="14">
+        <f>D42-Received!E42</f>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="11"/>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" s="14">
+        <f>60-Received!C43</f>
+        <v>26.21</v>
+      </c>
+      <c r="D43" s="14">
+        <f>C43-Received!D43</f>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="E43" s="14">
+        <f>D43-Received!E43</f>
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="11"/>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" s="14">
+        <f>60-Received!C44</f>
+        <v>48.29</v>
+      </c>
+      <c r="D44" s="14">
+        <f>C44-Received!D44</f>
+        <v>15.649999999999999</v>
+      </c>
+      <c r="E44" s="14">
+        <f>D44-Received!E44</f>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="11"/>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" s="14">
+        <f>60-Received!C45</f>
+        <v>57.32</v>
+      </c>
+      <c r="D45" s="14">
+        <f>C45-Received!D45</f>
+        <v>18.369999999999997</v>
+      </c>
+      <c r="E45" s="14">
+        <f>D45-Received!E45</f>
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="11"/>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" s="14">
+        <f>60-Received!C46</f>
+        <v>26.93</v>
+      </c>
+      <c r="D46" s="14">
+        <f>C46-Received!D46</f>
+        <v>19.54</v>
+      </c>
+      <c r="E46" s="14">
+        <f>D46-Received!E46</f>
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="11"/>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47" s="14">
+        <f>60-Received!C47</f>
+        <v>39.489999999999995</v>
+      </c>
+      <c r="D47" s="14">
+        <f>C47-Received!D47</f>
+        <v>7.9699999999999953</v>
+      </c>
+      <c r="E47" s="14">
+        <f>D47-Received!E47</f>
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="11"/>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48" s="14">
+        <f>60-Received!C48</f>
+        <v>40.21</v>
+      </c>
+      <c r="D48" s="14">
+        <f>C48-Received!D48</f>
+        <v>11.880000000000003</v>
+      </c>
+      <c r="E48" s="14">
+        <f>D48-Received!E48</f>
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="11"/>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49" s="14">
+        <f>60-Received!C49</f>
+        <v>53.71</v>
+      </c>
+      <c r="D49" s="14">
+        <f>C49-Received!D49</f>
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E49" s="14">
+        <f>D49-Received!E49</f>
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="11"/>
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="C50" s="14">
+        <f>60-Received!C50</f>
+        <v>43.8</v>
+      </c>
+      <c r="D50" s="14">
+        <f>C50-Received!D50</f>
+        <v>38.019999999999996</v>
+      </c>
+      <c r="E50" s="14">
+        <f>D50-Received!E50</f>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="11"/>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51" s="14">
+        <f>60-Received!C51</f>
+        <v>58</v>
+      </c>
+      <c r="D51" s="14">
+        <f>C51-Received!D51</f>
+        <v>52.53</v>
+      </c>
+      <c r="E51" s="14">
+        <f>D51-Received!E51</f>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="11"/>
+      <c r="B52">
+        <f t="shared" ref="B52:B61" si="0">B42+10</f>
+        <v>11</v>
+      </c>
+      <c r="C52" s="14">
+        <f>60-Received!C52</f>
+        <v>28.14</v>
+      </c>
+      <c r="D52" s="14">
+        <f>C52-Received!D52</f>
+        <v>3.6000000000000014</v>
+      </c>
+      <c r="E52" s="14">
+        <f>D52-Received!E52</f>
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="11"/>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C53" s="14">
+        <f>60-Received!C53</f>
+        <v>47.63</v>
+      </c>
+      <c r="D53" s="14">
+        <f>C53-Received!D53</f>
+        <v>38.650000000000006</v>
+      </c>
+      <c r="E53" s="14">
+        <f>D53-Received!E53</f>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="11"/>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C54" s="14">
+        <f>60-Received!C54</f>
+        <v>40.71</v>
+      </c>
+      <c r="D54" s="14">
+        <f>C54-Received!D54</f>
+        <v>17.55</v>
+      </c>
+      <c r="E54" s="14">
+        <f>D54-Received!E54</f>
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="11"/>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C55" s="14">
+        <f>60-Received!C55</f>
+        <v>42.85</v>
+      </c>
+      <c r="D55" s="14">
+        <f>C55-Received!D55</f>
+        <v>38.49</v>
+      </c>
+      <c r="E55" s="14">
+        <f>D55-Received!E55</f>
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="11"/>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C56" s="14">
+        <f>60-Received!C56</f>
+        <v>47.51</v>
+      </c>
+      <c r="D56" s="14">
+        <f>C56-Received!D56</f>
+        <v>25.939999999999998</v>
+      </c>
+      <c r="E56" s="14">
+        <f>D56-Received!E56</f>
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="11"/>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C57" s="14">
+        <f>60-Received!C57</f>
+        <v>21.840000000000003</v>
+      </c>
+      <c r="D57" s="14">
+        <f>C57-Received!D57</f>
+        <v>16.560000000000002</v>
+      </c>
+      <c r="E57" s="14">
+        <f>D57-Received!E57</f>
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="11"/>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C58" s="14">
+        <f>60-Received!C58</f>
+        <v>39.75</v>
+      </c>
+      <c r="D58" s="14">
+        <f>C58-Received!D58</f>
+        <v>33.49</v>
+      </c>
+      <c r="E58" s="14">
+        <f>D58-Received!E58</f>
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="11"/>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C59" s="14">
+        <f>60-Received!C59</f>
+        <v>28.22</v>
+      </c>
+      <c r="D59" s="14">
+        <f>C59-Received!D59</f>
+        <v>19.07</v>
+      </c>
+      <c r="E59" s="14">
+        <f>D59-Received!E59</f>
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="11"/>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C60" s="14">
+        <f>60-Received!C60</f>
+        <v>45.63</v>
+      </c>
+      <c r="D60" s="14">
+        <f>C60-Received!D60</f>
+        <v>12.300000000000004</v>
+      </c>
+      <c r="E60" s="14">
+        <f>D60-Received!E60</f>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="11"/>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C61" s="14">
+        <f>60-Received!C61</f>
+        <v>22.11</v>
+      </c>
+      <c r="D61" s="14">
+        <f>C61-Received!D61</f>
+        <v>4.59</v>
+      </c>
+      <c r="E61" s="14">
+        <f>D61-Received!E61</f>
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="A42:A61"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>